<commit_message>
[ATUALIZAÇÃO] Art 1 - Escopo
</commit_message>
<xml_diff>
--- a/Artefato 31 OPE - Requisitos de Software do Subsistema (SRS).xlsx
+++ b/Artefato 31 OPE - Requisitos de Software do Subsistema (SRS).xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan-AMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDF7FC0-B875-4ED8-88CA-DA380ED228CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{1FDF7FC0-B875-4ED8-88CA-DA380ED228CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9EC1D5B6-4702-4007-AED1-B322BAEAD8AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{722396AB-12E8-4CE8-96A8-58F6DF15ACC8}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{722396AB-12E8-4CE8-96A8-58F6DF15ACC8}"/>
   </bookViews>
   <sheets>
     <sheet name="modelo_01" sheetId="1" r:id="rId1"/>
-    <sheet name="modelo_02" sheetId="2" r:id="rId2"/>
+    <sheet name="modelo_01 Antigo" sheetId="3" r:id="rId2"/>
+    <sheet name="modelo_02" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>- (18) Descrição dos Processo de Negócio)</t>
   </si>
@@ -347,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -362,9 +363,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,6 +370,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -698,9 +702,188 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
+  <dimension ref="B4:E28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" display="http://walderson.com/IBM/RUP7/LargeProjects/core.base_rup/tasks/use_case_analysis_A6990185.html" xr:uid="{8334008F-AB75-4731-A362-68FFB946055D}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD70439E-31EA-4A5F-ADD5-4473C0372831}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="B4:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -733,13 +916,13 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="12"/>
       <c r="F8" s="2" t="s">
         <v>17</v>
       </c>
@@ -942,20 +1125,19 @@
   <mergeCells count="1">
     <mergeCell ref="C8:D8"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="http://walderson.com/IBM/RUP7/LargeProjects/core.base_rup/tasks/use_case_analysis_A6990185.html" xr:uid="{8334008F-AB75-4731-A362-68FFB946055D}"/>
+    <hyperlink ref="F8" r:id="rId1" display="http://walderson.com/IBM/RUP7/LargeProjects/core.base_rup/tasks/use_case_analysis_A6990185.html" xr:uid="{2BDFCCB9-DD57-42DC-9097-0E79E2834FE2}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB3D808-12A7-462D-99C0-0BA22A08B5CC}">
   <dimension ref="B1:D22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -968,13 +1150,13 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">

</xml_diff>